<commit_message>
tested a few matrix combinations
</commit_message>
<xml_diff>
--- a/first_transition_matrix_with_manual_edits.xlsx
+++ b/first_transition_matrix_with_manual_edits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ddb8727edf2838dd/Documents/Development/NCAA_Markov/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_4ED1509A995F200E62355476585DCE3A87472E5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E1057A-B7FA-482D-BF0F-D4C44C16F616}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_4ED1509A995F200E62355476585DCE3A87472E5F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5344B580-366C-472C-9439-ABDEFDC9AFD4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -200,10 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,9 +493,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -617,7 +613,7 @@
         <v>8.7476671292530034E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -676,7 +672,7 @@
         <v>0.18196397730076491</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -735,7 +731,7 @@
         <v>0.26605058365758749</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -794,7 +790,7 @@
         <v>0.21582733812949639</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -853,7 +849,7 @@
         <v>0.33828777327374149</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -912,7 +908,7 @@
         <v>0.38463516003256348</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -971,7 +967,7 @@
         <v>0.39688972014408419</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1030,7 +1026,7 @@
         <v>0.39649643229375447</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1089,7 +1085,7 @@
         <v>0.34778034444114081</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1148,7 +1144,7 @@
         <v>1.4157014157014159E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1207,7 +1203,7 @@
         <v>2.8488231011890321E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1262,7 @@
         <v>4.9592894152479652E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1325,7 +1321,7 @@
         <v>9.5435684647302899E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1384,7 +1380,7 @@
         <v>0.24375302831037579</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1443,7 +1439,7 @@
         <v>0.1323550883340634</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1502,7 +1498,7 @@
         <v>0.11291950340408489</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +1557,7 @@
         <v>0.10916343409207351</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1633,9 +1629,9 @@
       <selection sqref="A1:S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +1690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +1749,7 @@
         <v>8.7476671292530034E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1812,7 +1808,7 @@
         <v>0.18196397730076491</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1871,7 +1867,7 @@
         <v>0.26605058365758749</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1930,7 +1926,7 @@
         <v>0.21582733812949639</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1989,7 +1985,7 @@
         <v>0.33828777327374149</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2048,7 +2044,7 @@
         <v>0.38463516003256348</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2107,7 +2103,7 @@
         <v>0.39688972014408419</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2166,7 +2162,7 @@
         <v>0.39649643229375447</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2225,7 +2221,7 @@
         <v>0.34778034444114081</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2284,7 +2280,7 @@
         <v>1.4157014157014159E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2343,7 +2339,7 @@
         <v>2.8488231011890321E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2402,7 +2398,7 @@
         <v>4.9592894152479652E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2461,7 +2457,7 @@
         <v>9.5435684647302899E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2520,7 +2516,7 @@
         <v>0.24375302831037579</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>0.1323550883340634</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -2638,7 +2634,7 @@
         <v>0.11291950340408489</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -2697,7 +2693,7 @@
         <v>0.10916343409207351</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2756,7 +2752,7 @@
         <v>0.11650188691014569</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -2778,9 +2774,9 @@
       <selection activeCell="A10" sqref="A2:S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2839,7 +2835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2898,7 +2894,7 @@
         <v>1.7897305833373209E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2957,7 +2953,7 @@
         <v>3.4912410560078953E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3016,7 +3012,7 @@
         <v>5.7717250324254218E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3075,7 +3071,7 @@
         <v>9.7122302158273388E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -3134,7 +3130,7 @@
         <v>0.26185774174548732</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -3193,7 +3189,7 @@
         <v>0.13860919490980761</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -3252,7 +3248,7 @@
         <v>0.11885217511776119</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3311,7 +3307,7 @@
         <v>0.11729335364387081</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3370,7 +3366,7 @@
         <v>0.12514580426777669</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -3429,7 +3425,7 @@
         <v>9.682630959226704E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3484,7 @@
         <v>0.19966027663188551</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -3547,7 +3543,7 @@
         <v>0.27757216876387858</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -3606,7 +3602,7 @@
         <v>0.26970954356846472</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -3665,7 +3661,7 @@
         <v>0.37713712189381882</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -3724,7 +3720,7 @@
         <v>0.42210541684917507</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -3783,7 +3779,7 @@
         <v>0.44137765318382061</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -3842,7 +3838,7 @@
         <v>0.43811754373124501</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -3914,9 +3910,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3975,7 +3971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4034,7 +4030,7 @@
         <v>9.682630959226704E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -4093,7 +4089,7 @@
         <v>0.19966027663188551</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -4152,7 +4148,7 @@
         <v>0.27757216876387858</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -4211,7 +4207,7 @@
         <v>0.26970954356846472</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4270,7 +4266,7 @@
         <v>0.37713712189381882</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -4329,7 +4325,7 @@
         <v>0.42210541684917507</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -4388,7 +4384,7 @@
         <v>0.44137765318382061</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -4447,7 +4443,7 @@
         <v>0.43811754373124501</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -4506,7 +4502,7 @@
         <v>0.38786139787293772</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -4565,7 +4561,7 @@
         <v>1.7897305833373209E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -4624,7 +4620,7 @@
         <v>3.4912410560078953E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -4683,7 +4679,7 @@
         <v>5.7717250324254218E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -4742,7 +4738,7 @@
         <v>9.7122302158273388E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -4801,7 +4797,7 @@
         <v>0.26185774174548732</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -4860,7 +4856,7 @@
         <v>0.13860919490980761</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -4919,7 +4915,7 @@
         <v>0.11885217511776119</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -4978,7 +4974,7 @@
         <v>0.11729335364387081</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -5050,9 +5046,9 @@
       <selection activeCell="S19" sqref="A1:S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5111,7 +5107,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -5188,7 +5184,7 @@
         <v>9.2151490442398537E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -5265,7 +5261,7 @@
         <v>0.19081212696632521</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -5342,7 +5338,7 @@
         <v>0.27181137621073304</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5419,7 +5415,7 @@
         <v>0.24276844084898055</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -5496,7 +5492,7 @@
         <v>0.35771244758378018</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -5573,7 +5569,7 @@
         <v>0.40337028844086931</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -5650,7 +5646,7 @@
         <v>0.4191336866639524</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -5727,7 +5723,7 @@
         <v>0.41730698801249977</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -5804,7 +5800,7 @@
         <v>0.36782087115703926</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -5881,7 +5877,7 @@
         <v>1.6027159995193684E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -5958,7 +5954,7 @@
         <v>3.1700320785984636E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -6035,7 +6031,7 @@
         <v>5.3655072238366935E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -6112,7 +6108,7 @@
         <v>9.6278993402788143E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -6189,7 +6185,7 @@
         <v>0.25280538502793154</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -6266,7 +6262,7 @@
         <v>0.1354821416219355</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -6343,7 +6339,7 @@
         <v>0.11588583926092305</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -6420,7 +6416,7 @@
         <v>0.11322839386797215</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -6506,13 +6502,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3FF047-2998-4146-8045-EF0865912DDA}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6571,7 +6567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6630,7 +6626,7 @@
         <v>9.2151490442398537E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -6689,7 +6685,7 @@
         <v>0.19081212696632521</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6748,7 +6744,7 @@
         <v>0.27181137621073304</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -6807,7 +6803,7 @@
         <v>0.24276844084898055</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6866,7 +6862,7 @@
         <v>0.35771244758378018</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -6925,7 +6921,7 @@
         <v>0.40337028844086931</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6984,7 +6980,7 @@
         <v>0.4191336866639524</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -7043,7 +7039,7 @@
         <v>0.41730698801249977</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -7102,7 +7098,7 @@
         <v>0.36782087115703926</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -7161,7 +7157,7 @@
         <v>1.6027159995193684E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7220,7 +7216,7 @@
         <v>3.1700320785984636E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -7279,7 +7275,7 @@
         <v>5.3655072238366935E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -7338,7 +7334,7 @@
         <v>9.6278993402788143E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -7397,7 +7393,7 @@
         <v>0.25280538502793154</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -7456,7 +7452,7 @@
         <v>0.1354821416219355</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -7515,7 +7511,7 @@
         <v>0.11588583926092305</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -7574,7 +7570,7 @@
         <v>0.11322839386797215</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -7642,16 +7638,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17E5F4F-4F48-4BE8-AC81-BFF8850E5ED6}">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S19" sqref="B2:S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7710,7 +7706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7769,7 +7765,7 @@
         <v>9.2151490442398537E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -7828,7 +7824,7 @@
         <v>0.19081212696632521</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7887,7 +7883,7 @@
         <v>0.27181137621073304</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -7946,7 +7942,7 @@
         <v>0.24276844084898055</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8005,7 +8001,7 @@
         <v>0.35771244758378018</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8064,7 +8060,7 @@
         <v>0.40337028844086931</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -8123,7 +8119,7 @@
         <v>0.4191336866639524</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -8182,7 +8178,7 @@
         <v>0.41730698801249977</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -8241,7 +8237,7 @@
         <v>0.36782087115703926</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -8300,7 +8296,7 @@
         <v>1.6027159995193684E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -8359,7 +8355,7 @@
         <v>3.1700320785984636E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -8418,7 +8414,7 @@
         <v>5.3655072238366935E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -8477,7 +8473,7 @@
         <v>9.6278993402788143E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -8536,7 +8532,7 @@
         <v>0.25280538502793154</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -8595,7 +8591,7 @@
         <v>0.1354821416219355</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -8654,7 +8650,7 @@
         <v>0.11588583926092305</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -8713,7 +8709,7 @@
         <v>0.11322839386797215</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -8772,7 +8768,7 @@
         <v>0.1208238455889612</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>20</v>
       </c>
@@ -8780,12 +8776,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>23</v>
       </c>

</xml_diff>